<commit_message>
add example values to templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/DNA_extraction.xlsx
+++ b/templates/dataplant/DNA_extraction.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -200,7 +200,22 @@
     <t/>
   </si>
   <si>
-    <t>RNA (Transcriptomics)</t>
+    <t>Total RNA</t>
+  </si>
+  <si>
+    <t>https://bioregistry.io/NCIT:C163995</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>milligram</t>
+  </si>
+  <si>
+    <t>UO</t>
+  </si>
+  <si>
+    <t>https://bioregistry.io/UO:0000022</t>
   </si>
   <si>
     <t>QIAGEN RNEasy</t>
@@ -209,22 +224,10 @@
     <t>QIAGEN RNEasy Buffer 2</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>DNA (Genomics)</t>
-  </si>
-  <si>
-    <t>PCI method</t>
-  </si>
-  <si>
-    <t>phenol:chloroform:isopropanol</t>
-  </si>
-  <si>
-    <t>Metabolites</t>
-  </si>
-  <si>
-    <t>protein</t>
+    <t>microliter</t>
+  </si>
+  <si>
+    <t>https://bioregistry.io/UO:0000101</t>
   </si>
 </sst>
 </file>
@@ -280,8 +283,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:S5" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:S5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:S2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:S2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -815,7 +818,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -885,25 +888,25 @@
         <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="J2" t="s">
         <v>61</v>
@@ -912,7 +915,7 @@
         <v>61</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="M2" t="s">
         <v>61</v>
@@ -921,195 +924,18 @@
         <v>61</v>
       </c>
       <c r="O2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="Q2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="R2" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="S2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" t="s">
-        <v>68</v>
-      </c>
-      <c r="M3" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" t="s">
-        <v>61</v>
-      </c>
-      <c r="O3" t="s">
-        <v>61</v>
-      </c>
-      <c r="P3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R3" t="s">
-        <v>61</v>
-      </c>
-      <c r="S3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L4" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" t="s">
-        <v>61</v>
-      </c>
-      <c r="N4" t="s">
-        <v>61</v>
-      </c>
-      <c r="O4" t="s">
-        <v>61</v>
-      </c>
-      <c r="P4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>61</v>
-      </c>
-      <c r="R4" t="s">
-        <v>61</v>
-      </c>
-      <c r="S4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M5" t="s">
-        <v>61</v>
-      </c>
-      <c r="N5" t="s">
-        <v>61</v>
-      </c>
-      <c r="O5" t="s">
-        <v>61</v>
-      </c>
-      <c r="P5" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>61</v>
-      </c>
-      <c r="R5" t="s">
-        <v>61</v>
-      </c>
-      <c r="S5" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update DNA extraction example values and ontology ref for sample description
</commit_message>
<xml_diff>
--- a/templates/dataplant/DNA_extraction.xlsx
+++ b/templates/dataplant/DNA_extraction.xlsx
@@ -200,37 +200,37 @@
     <t/>
   </si>
   <si>
-    <t>total RNA</t>
-  </si>
-  <si>
-    <t>EFO</t>
-  </si>
-  <si>
-    <t>https://bioregistry.io/EFO:0004964</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>milligram</t>
+    <t>BAO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/BAO_0000269</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>gram</t>
   </si>
   <si>
     <t>UO</t>
   </si>
   <si>
-    <t>https://bioregistry.io/UO:0000022</t>
-  </si>
-  <si>
-    <t>QIAGEN RNEasy</t>
-  </si>
-  <si>
-    <t>QIAGEN RNEasy Buffer 2</t>
-  </si>
-  <si>
-    <t>microliter</t>
-  </si>
-  <si>
-    <t>https://bioregistry.io/UO:0000101</t>
+    <t>https://bioregistry.io/UO:0000021</t>
+  </si>
+  <si>
+    <t>Macherey Nagel NucleoBond HMW DNA Kit</t>
+  </si>
+  <si>
+    <t>Lysis buffer H1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>milliliter</t>
+  </si>
+  <si>
+    <t>https://bioregistry.io/UO:0000098</t>
   </si>
 </sst>
 </file>
@@ -888,28 +888,28 @@
         <v>61</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>65</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>66</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>67</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>68</v>
-      </c>
-      <c r="I2" t="s">
-        <v>69</v>
       </c>
       <c r="J2" t="s">
         <v>61</v>
@@ -918,7 +918,7 @@
         <v>61</v>
       </c>
       <c r="L2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M2" t="s">
         <v>61</v>
@@ -927,13 +927,13 @@
         <v>61</v>
       </c>
       <c r="O2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="P2" t="s">
         <v>71</v>
       </c>
       <c r="Q2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R2" t="s">
         <v>72</v>

</xml_diff>